<commit_message>
remove alive_progress - no longer works in docker
</commit_message>
<xml_diff>
--- a/manifest_templates/files_manifest.xlsx
+++ b/manifest_templates/files_manifest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10314"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vchung/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vchung/Desktop/csbc-pson-dcc/manifest_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A3275F5-6D99-5446-8022-2AF1B1F02F2F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7EFAD62-80AF-8946-9026-46AD6A1A8BD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2720" yWindow="500" windowWidth="26080" windowHeight="17500" xr2:uid="{699C1E4D-FBE1-2149-B5D3-FBE286AFA841}"/>
+    <workbookView xWindow="2720" yWindow="500" windowWidth="40540" windowHeight="17500" xr2:uid="{699C1E4D-FBE1-2149-B5D3-FBE286AFA841}"/>
   </bookViews>
   <sheets>
     <sheet name="manifest" sheetId="1" r:id="rId1"/>
@@ -2252,54 +2252,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="7">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Value is not one of the acceptable values for this column. Please see `standard_terms` tab for more information." prompt="Select value from the dropdown list." xr:uid="{65498581-D402-2941-BA11-D491DC8E7647}">
-          <x14:formula1>
-            <xm:f>standard_terms!$B$235:$B$261</xm:f>
-          </x14:formula1>
-          <xm:sqref>G2:G1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Value is not one of the acceptable values for this column. Please see `standard_terms` tab for more information." prompt="Select value from the dropdown list." xr:uid="{79C9852E-8342-A140-A692-3F8534689EB4}">
-          <x14:formula1>
-            <xm:f>standard_terms!$B$194:$B$234</xm:f>
-          </x14:formula1>
-          <xm:sqref>H2:H1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Value is not one of the acceptable values for this column. Please see `standard_terms` tab for more information." prompt="Select value from the dropdown list." xr:uid="{DCDE5A15-720E-844B-9284-441A30410061}">
-          <x14:formula1>
-            <xm:f>standard_terms!$B$267:$B$279</xm:f>
-          </x14:formula1>
-          <xm:sqref>I2:I1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Value is not one of the acceptable values for this column. Please see `standard_terms` tab for more information." prompt="Select value from the dropdown list." xr:uid="{3EA22FF0-3EEA-AA4A-BD8C-E961D625194B}">
-          <x14:formula1>
-            <xm:f>standard_terms!$B$262:$B$266</xm:f>
-          </x14:formula1>
-          <xm:sqref>J2:J1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Value is not one of the acceptable values for this column. Please see `standard_terms` tab for more information." prompt="Select value from the dropdown list." xr:uid="{B068EA18-B2A9-0740-96B2-0E9839D88E4F}">
-          <x14:formula1>
-            <xm:f>standard_terms!$B$2:$B$193</xm:f>
-          </x14:formula1>
-          <xm:sqref>F2:F1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Value is not one of the acceptable values for this column. Please see `standard_terms` tab for more information." prompt="Select value from the dropdown list." xr:uid="{6AFE858B-80E4-9C42-9188-F2366CF608D0}">
-          <x14:formula1>
-            <xm:f>standard_terms!$B$417:$B$566</xm:f>
-          </x14:formula1>
-          <xm:sqref>K2:K1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Value is not one of the acceptable values for this column. Please see `standard_terms` tab for more information." prompt="Select value from the dropdown list." xr:uid="{BA2301E7-B7B5-AB49-B6E9-6950BB57B987}">
-          <x14:formula1>
-            <xm:f>standard_terms!$B$280:$B$416</xm:f>
-          </x14:formula1>
-          <xm:sqref>L2:L1048576</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 

</xml_diff>